<commit_message>
new corona report numbers #53
</commit_message>
<xml_diff>
--- a/data/kbvreport_export/impftabelle_vorschlag.xlsx
+++ b/data/kbvreport_export/impftabelle_vorschlag.xlsx
@@ -41,73 +41,73 @@
     <t xml:space="preserve">Gesamt</t>
   </si>
   <si>
+    <t xml:space="preserve">0,8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Schleswig-Holstein</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hamburg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Niedersachsen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0,7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bremen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nordrhein-Westfalen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hessen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0,9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rheinland-Pfalz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Baden-Württemberg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bayern</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Saarland</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Berlin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brandenburg</t>
+  </si>
+  <si>
     <t xml:space="preserve">0,6</t>
   </si>
   <si>
-    <t xml:space="preserve">Schleswig-Holstein</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1,0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hamburg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0,5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Niedersachsen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bremen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0,8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nordrhein-Westfalen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hessen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rheinland-Pfalz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Baden-Württemberg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bayern</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0,7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Saarland</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Berlin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Brandenburg</t>
-  </si>
-  <si>
     <t xml:space="preserve">Mecklenburg-Vorpommern</t>
   </si>
   <si>
-    <t xml:space="preserve">1,6</t>
+    <t xml:space="preserve">1,7</t>
   </si>
   <si>
     <t xml:space="preserve">Sachsen</t>
   </si>
   <si>
-    <t xml:space="preserve">0,4</t>
-  </si>
-  <si>
     <t xml:space="preserve">Sachsen-Anhalt</t>
   </si>
   <si>
-    <t xml:space="preserve">0,9</t>
+    <t xml:space="preserve">1,1</t>
   </si>
   <si>
     <t xml:space="preserve">Thüringen</t>
@@ -476,22 +476,22 @@
         <v>9</v>
       </c>
       <c r="C2" t="n">
-        <v>174</v>
+        <v>157</v>
       </c>
       <c r="D2" t="n">
-        <v>331</v>
+        <v>309</v>
       </c>
       <c r="E2" t="n">
-        <v>532878</v>
+        <v>688782</v>
       </c>
       <c r="F2" t="n">
-        <v>2.31728413547579</v>
+        <v>2.35087810554394</v>
       </c>
       <c r="G2" t="n">
-        <v>26.0117722982399</v>
+        <v>32.9869659348083</v>
       </c>
       <c r="H2" t="n">
-        <v>2.15840672682483</v>
+        <v>2.92784804444886</v>
       </c>
     </row>
     <row r="3">
@@ -502,22 +502,22 @@
         <v>11</v>
       </c>
       <c r="C3" t="n">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="D3" t="n">
-        <v>199</v>
+        <v>210</v>
       </c>
       <c r="E3" t="n">
-        <v>28241</v>
+        <v>38426</v>
       </c>
       <c r="F3" t="n">
-        <v>0.9859241752024</v>
+        <v>1.00651807148837</v>
       </c>
       <c r="G3" t="n">
-        <v>30.878866809096</v>
+        <v>47.0602007667769</v>
       </c>
       <c r="H3" t="n">
-        <v>3.12340482909399</v>
+        <v>5.45319708366641</v>
       </c>
     </row>
     <row r="4">
@@ -525,51 +525,51 @@
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C4" t="n">
-        <v>163</v>
+        <v>119</v>
       </c>
       <c r="D4" t="n">
-        <v>341</v>
+        <v>236</v>
       </c>
       <c r="E4" t="n">
-        <v>9888</v>
+        <v>14273</v>
       </c>
       <c r="F4" t="n">
-        <v>2.22508773838776</v>
+        <v>2.23770106206351</v>
       </c>
       <c r="G4" t="n">
-        <v>16.4173403781272</v>
+        <v>23.3942326055128</v>
       </c>
       <c r="H4" t="n">
-        <v>2.94497210075295</v>
+        <v>4.59014567027825</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
         <v>14</v>
       </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
       <c r="C5" t="n">
-        <v>131</v>
+        <v>113</v>
       </c>
       <c r="D5" t="n">
-        <v>238</v>
+        <v>212</v>
       </c>
       <c r="E5" t="n">
-        <v>41646</v>
+        <v>54168</v>
       </c>
       <c r="F5" t="n">
-        <v>1.52144063106422</v>
+        <v>1.53656521560727</v>
       </c>
       <c r="G5" t="n">
-        <v>24.2223983548263</v>
+        <v>31.1758279422475</v>
       </c>
       <c r="H5" t="n">
-        <v>1.69003261371508</v>
+        <v>2.12277764950358</v>
       </c>
     </row>
     <row r="6">
@@ -580,22 +580,22 @@
         <v>16</v>
       </c>
       <c r="C6" t="n">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="D6" t="n">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="E6" t="n">
-        <v>5291</v>
+        <v>6999</v>
       </c>
       <c r="F6" t="n">
-        <v>2.10862563527412</v>
+        <v>2.12580115736595</v>
       </c>
       <c r="G6" t="n">
-        <v>32.3796701447324</v>
+        <v>45.9946146078761</v>
       </c>
       <c r="H6" t="n">
-        <v>2.31536399982426</v>
+        <v>2.35710206054216</v>
       </c>
     </row>
     <row r="7">
@@ -603,22 +603,22 @@
         <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="D7" t="n">
-        <v>262</v>
+        <v>248</v>
       </c>
       <c r="E7" t="n">
-        <v>98950</v>
+        <v>124637</v>
       </c>
       <c r="F7" t="n">
-        <v>2.39712878110767</v>
+        <v>2.42648708677516</v>
       </c>
       <c r="G7" t="n">
-        <v>33.7710966275937</v>
+        <v>41.2788389295771</v>
       </c>
       <c r="H7" t="n">
         <v>0</v>
@@ -629,103 +629,103 @@
         <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C8" t="n">
-        <v>166</v>
+        <v>150</v>
       </c>
       <c r="D8" t="n">
-        <v>360</v>
+        <v>339</v>
       </c>
       <c r="E8" t="n">
-        <v>48653</v>
+        <v>57475</v>
       </c>
       <c r="F8" t="n">
-        <v>2.40149616417094</v>
+        <v>2.4300263355428</v>
       </c>
       <c r="G8" t="n">
-        <v>32.9119892638871</v>
+        <v>40.0047151847083</v>
       </c>
       <c r="H8" t="n">
-        <v>3.11207581446346</v>
+        <v>3.79047567190296</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" t="s">
         <v>19</v>
       </c>
-      <c r="B9" t="s">
-        <v>9</v>
-      </c>
       <c r="C9" t="n">
-        <v>146</v>
+        <v>133</v>
       </c>
       <c r="D9" t="n">
-        <v>318</v>
+        <v>286</v>
       </c>
       <c r="E9" t="n">
-        <v>25482</v>
+        <v>36466</v>
       </c>
       <c r="F9" t="n">
-        <v>1.97271405795399</v>
+        <v>1.99733603849432</v>
       </c>
       <c r="G9" t="n">
-        <v>20.9607107383291</v>
+        <v>27.825295221278</v>
       </c>
       <c r="H9" t="n">
-        <v>1.33920973506552</v>
+        <v>2.51567198048448</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C10" t="n">
-        <v>144</v>
+        <v>129</v>
       </c>
       <c r="D10" t="n">
-        <v>248</v>
+        <v>214</v>
       </c>
       <c r="E10" t="n">
-        <v>55320</v>
+        <v>73776</v>
       </c>
       <c r="F10" t="n">
-        <v>2.35687129664046</v>
+        <v>2.38435680751512</v>
       </c>
       <c r="G10" t="n">
-        <v>10.0205917654961</v>
+        <v>12.4717826742867</v>
       </c>
       <c r="H10" t="n">
-        <v>4.06352671293558</v>
+        <v>5.32842316333814</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C11" t="n">
-        <v>166</v>
+        <v>149</v>
       </c>
       <c r="D11" t="n">
-        <v>317</v>
+        <v>291</v>
       </c>
       <c r="E11" t="n">
-        <v>93966</v>
+        <v>135986</v>
       </c>
       <c r="F11" t="n">
-        <v>2.7240622040655</v>
+        <v>2.75576569648596</v>
       </c>
       <c r="G11" t="n">
-        <v>28.0447393903858</v>
+        <v>39.7244209909118</v>
       </c>
       <c r="H11" t="n">
-        <v>2.4852705775954</v>
+        <v>3.8101068071038</v>
       </c>
     </row>
     <row r="12">
@@ -736,22 +736,22 @@
         <v>16</v>
       </c>
       <c r="C12" t="n">
-        <v>176</v>
+        <v>182</v>
       </c>
       <c r="D12" t="n">
-        <v>356</v>
+        <v>388</v>
       </c>
       <c r="E12" t="n">
-        <v>8232</v>
+        <v>10130</v>
       </c>
       <c r="F12" t="n">
-        <v>2.22720534367157</v>
+        <v>2.26358235542671</v>
       </c>
       <c r="G12" t="n">
-        <v>25.7606313020605</v>
+        <v>30.9951775537045</v>
       </c>
       <c r="H12" t="n">
-        <v>8.22745563691536</v>
+        <v>10.1009301405106</v>
       </c>
     </row>
     <row r="13">
@@ -759,25 +759,25 @@
         <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C13" t="n">
-        <v>204</v>
+        <v>191</v>
       </c>
       <c r="D13" t="n">
-        <v>463</v>
+        <v>438</v>
       </c>
       <c r="E13" t="n">
-        <v>28871</v>
+        <v>33798</v>
       </c>
       <c r="F13" t="n">
-        <v>2.91157547463667</v>
+        <v>2.958012432787</v>
       </c>
       <c r="G13" t="n">
-        <v>63.0237236403996</v>
+        <v>70.8310210876804</v>
       </c>
       <c r="H13" t="n">
-        <v>8.80143163516028</v>
+        <v>10.7154861831111</v>
       </c>
     </row>
     <row r="14">
@@ -785,77 +785,77 @@
         <v>25</v>
       </c>
       <c r="B14" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="C14" t="n">
-        <v>289</v>
+        <v>260</v>
       </c>
       <c r="D14" t="n">
-        <v>454</v>
+        <v>456</v>
       </c>
       <c r="E14" t="n">
-        <v>13895</v>
+        <v>15091</v>
       </c>
       <c r="F14" t="n">
-        <v>2.02768317291812</v>
+        <v>2.10353888923915</v>
       </c>
       <c r="G14" t="n">
-        <v>3.73939543694918</v>
+        <v>4.78543777283585</v>
       </c>
       <c r="H14" t="n">
-        <v>0.814812562707124</v>
+        <v>1.22931298328823</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B15" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C15" t="n">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="D15" t="n">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="E15" t="n">
-        <v>25141</v>
+        <v>26926</v>
       </c>
       <c r="F15" t="n">
-        <v>0.917458576316212</v>
+        <v>0.952343642150114</v>
       </c>
       <c r="G15" t="n">
-        <v>60.3893045889802</v>
+        <v>64.4183977813825</v>
       </c>
       <c r="H15" t="n">
-        <v>1.16273562565123</v>
+        <v>1.2598276025386</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B16" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C16" t="n">
-        <v>375</v>
+        <v>309</v>
       </c>
       <c r="D16" t="n">
-        <v>696</v>
+        <v>633</v>
       </c>
       <c r="E16" t="n">
-        <v>17991</v>
+        <v>23701</v>
       </c>
       <c r="F16" t="n">
-        <v>3.83656956299541</v>
+        <v>3.8995366126134</v>
       </c>
       <c r="G16" t="n">
-        <v>5.38203073741973</v>
+        <v>9.00053681134064</v>
       </c>
       <c r="H16" t="n">
-        <v>0.293614178353409</v>
+        <v>0.517552335867094</v>
       </c>
     </row>
     <row r="17">
@@ -866,22 +866,22 @@
         <v>31</v>
       </c>
       <c r="C17" t="n">
-        <v>229</v>
+        <v>235</v>
       </c>
       <c r="D17" t="n">
-        <v>455</v>
+        <v>473</v>
       </c>
       <c r="E17" t="n">
-        <v>20799</v>
+        <v>24413</v>
       </c>
       <c r="F17" t="n">
-        <v>1.71233407235889</v>
+        <v>1.79061063923433</v>
       </c>
       <c r="G17" t="n">
-        <v>36.0485635632103</v>
+        <v>41.134326251147</v>
       </c>
       <c r="H17" t="n">
-        <v>3.52813947871149</v>
+        <v>4.15669396807273</v>
       </c>
     </row>
     <row r="18">
@@ -889,25 +889,25 @@
         <v>32</v>
       </c>
       <c r="B18" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="C18" t="n">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="D18" t="n">
-        <v>589</v>
+        <v>582</v>
       </c>
       <c r="E18" t="n">
-        <v>10512</v>
+        <v>12517</v>
       </c>
       <c r="F18" t="n">
-        <v>2.43013661901454</v>
+        <v>2.50888497022094</v>
       </c>
       <c r="G18" t="n">
-        <v>3.696</v>
+        <v>4.996</v>
       </c>
       <c r="H18" t="n">
-        <v>0.532799943356817</v>
+        <v>0.63369561369349</v>
       </c>
     </row>
   </sheetData>

</xml_diff>